<commit_message>
added oversampling to extra trees model
</commit_message>
<xml_diff>
--- a/spring21_models/y_v3.xlsx
+++ b/spring21_models/y_v3.xlsx
@@ -374,7 +374,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B252"/>
+  <dimension ref="A1:B395"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -419,223 +419,223 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>0.06054918107232599</v>
+        <v>0.01498356755149082</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>0.01648193705320629</v>
+        <v>0.06054918107232599</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>0.04248855464559233</v>
+        <v>0.01648193705320629</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>0.01725185286986227</v>
+        <v>0.04248855464559233</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>0.06727687122198339</v>
+        <v>0.02217199926699652</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>0.05978139638634843</v>
+        <v>0.01725185286986227</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>0.05239522468791943</v>
+        <v>0.06727687122198339</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>0.01858708081363386</v>
+        <v>0.05978139638634843</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>0.06506059930106327</v>
+        <v>0.05239522468791943</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>0.111006831965931</v>
+        <v>0.01116345346972159</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>0.2349271852394761</v>
+        <v>0.01858708081363386</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>0.10091530178721</v>
+        <v>0.002655332600329852</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>0.04248855464559233</v>
+        <v>0.02748763056624519</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>0.111006831965931</v>
+        <v>0.06506059930106327</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>0.1965095652358646</v>
+        <v>0.1914223168971915</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>0.1177983488598102</v>
+        <v>0.111006831965931</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>0.3288980593352666</v>
+        <v>0.04367614261350448</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>0.1658993413108993</v>
+        <v>0.02136331526949432</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>0.05889917442990508</v>
+        <v>0.2349271852394761</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>0.04319272791526372</v>
+        <v>0.10091530178721</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>0.1857260304901393</v>
+        <v>0.04248855464559233</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>0.0857225178717483</v>
+        <v>0.111006831965931</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>0.0638074389657305</v>
+        <v>0.1965095652358646</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>0.2944958721495254</v>
+        <v>0.1177983488598102</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>0.08497710929118467</v>
+        <v>0.3288980593352666</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>0.050457650893605</v>
+        <v>0.1658993413108993</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>0.251298118171377</v>
+        <v>0.05889917442990508</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>0.01484849585742686</v>
@@ -643,1753 +643,2897 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>0.09054057174271578</v>
+        <v>0.09423867908784812</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>0.02011290086127909</v>
+        <v>0.01858708081363386</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>0.08834876164485761</v>
+        <v>0.06373283196838851</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>0.05893041964449331</v>
+        <v>0.08497710929118467</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>0.01648193705320629</v>
+        <v>0.04319272791526372</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>0.1416961440263187</v>
+        <v>0.1857260304901393</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>0.03078295784073165</v>
+        <v>0.0857225178717483</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B41">
-        <v>0.07271859996334983</v>
+        <v>0.01078886374982739</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="B42">
-        <v>0.008230804471321239</v>
+        <v>0.0638074389657305</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="B43">
-        <v>0.1670898314266595</v>
+        <v>0.08896041128920898</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="B44">
-        <v>0.04367373783977462</v>
+        <v>0.1805763572437675</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="B45">
-        <v>0.04657629701391622</v>
+        <v>0.2944958721495254</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="B46">
-        <v>0.07703866593366318</v>
+        <v>0.08497710929118467</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="B47">
-        <v>0.1495041526646685</v>
+        <v>0.050457650893605</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="B48">
-        <v>0.1911984959051655</v>
+        <v>0.251298118171377</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="B49">
-        <v>0.05239522468791943</v>
+        <v>0.02136332233828111</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="B50">
-        <v>0.1699542185823693</v>
+        <v>0.03067665334890889</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="B51">
-        <v>0.01397287105785879</v>
+        <v>0.01484849585742686</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="B52">
-        <v>0.05978139638634843</v>
+        <v>0.01484849585742686</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="B53">
-        <v>0.01648193705320629</v>
+        <v>0.09054057174271578</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="B54">
-        <v>0.001798497342862378</v>
+        <v>0.1766975232897152</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="B55">
-        <v>0.009816529071650846</v>
+        <v>0.002634194788778773</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1">
-        <v>103</v>
+        <v>54</v>
       </c>
       <c r="B56">
-        <v>0.07198787658659651</v>
+        <v>0.02011290086127909</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="B57">
-        <v>0.1990096342797659</v>
+        <v>0.01538256977098038</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="B58">
-        <v>0.02349966132974703</v>
+        <v>0.08834876164485761</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="B59">
-        <v>0.221679423855199</v>
+        <v>0.05893041964449331</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1">
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="B60">
-        <v>0.1177983488598102</v>
+        <v>0.01648193705320629</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="B61">
-        <v>0.2212545995968481</v>
+        <v>0.1416961440263187</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="B62">
-        <v>0.252288254468025</v>
+        <v>0.01858708081363386</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1">
-        <v>114</v>
+        <v>61</v>
       </c>
       <c r="B63">
-        <v>0.2349271852394761</v>
+        <v>0.03078295784073165</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="B64">
-        <v>0.07330034817665385</v>
+        <v>0.0197821971779366</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="B65">
-        <v>0.01369126981724239</v>
+        <v>0.05098312538652583</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="B66">
-        <v>0.05978139638634843</v>
+        <v>0.02349966132974703</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="B67">
-        <v>0.0252288254468025</v>
+        <v>0.02867977438577483</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="B68">
-        <v>0.1001039270046631</v>
+        <v>0.01078886374982739</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1">
-        <v>122</v>
+        <v>67</v>
       </c>
       <c r="B69">
-        <v>0.02349966098588968</v>
+        <v>0.07271859996334983</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1">
-        <v>124</v>
+        <v>68</v>
       </c>
       <c r="B70">
-        <v>0.03320113428799209</v>
+        <v>0.008230804471321239</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="1">
-        <v>126</v>
+        <v>69</v>
       </c>
       <c r="B71">
-        <v>0.20183060357442</v>
+        <v>0.01078886374982739</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="1">
-        <v>128</v>
+        <v>70</v>
       </c>
       <c r="B72">
-        <v>0.191739073395699</v>
+        <v>0.1168435252753789</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="1">
-        <v>129</v>
+        <v>71</v>
       </c>
       <c r="B73">
-        <v>0.03282010262048745</v>
+        <v>0.015382572842221</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="1">
-        <v>131</v>
+        <v>72</v>
       </c>
       <c r="B74">
-        <v>0.2565512186182884</v>
+        <v>0.01538256990907531</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="1">
-        <v>132</v>
+        <v>73</v>
       </c>
       <c r="B75">
-        <v>0.02650462849345728</v>
+        <v>0.01249953074384669</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="1">
-        <v>133</v>
+        <v>74</v>
       </c>
       <c r="B76">
-        <v>0.03665017408832692</v>
+        <v>0.1327767332674761</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="1">
-        <v>134</v>
+        <v>75</v>
       </c>
       <c r="B77">
-        <v>0.1145317940260216</v>
+        <v>0.1670898314266595</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="1">
-        <v>135</v>
+        <v>76</v>
       </c>
       <c r="B78">
-        <v>0.0488405935651084</v>
+        <v>0.02261950151665374</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="1">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="B79">
-        <v>0.04225928168488188</v>
+        <v>0.007857951621204324</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="1">
-        <v>139</v>
+        <v>78</v>
       </c>
       <c r="B80">
-        <v>0.3</v>
+        <v>0.022200269802322</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="1">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="B81">
-        <v>0.07330034817665385</v>
+        <v>0.04367373783977462</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="1">
-        <v>141</v>
+        <v>80</v>
       </c>
       <c r="B82">
-        <v>0.01484849585742686</v>
+        <v>0.0135295526607702</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="1">
-        <v>144</v>
+        <v>81</v>
       </c>
       <c r="B83">
-        <v>0.09559924795258276</v>
+        <v>0.03540295083012013</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="1">
-        <v>145</v>
+        <v>82</v>
       </c>
       <c r="B84">
-        <v>0.02125750412314458</v>
+        <v>0.04657629701391622</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="1">
-        <v>146</v>
+        <v>83</v>
       </c>
       <c r="B85">
-        <v>0.2464336169444356</v>
+        <v>0.01992228253933974</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="1">
-        <v>150</v>
+        <v>84</v>
       </c>
       <c r="B86">
-        <v>0.1301211986021265</v>
+        <v>0.07703866593366318</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="1">
-        <v>152</v>
+        <v>85</v>
       </c>
       <c r="B87">
-        <v>0.2804054242257651</v>
+        <v>0.001798497342862378</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="1">
-        <v>153</v>
+        <v>86</v>
       </c>
       <c r="B88">
-        <v>0.06818636613523914</v>
+        <v>0.1194057763190041</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="1">
-        <v>154</v>
+        <v>87</v>
       </c>
       <c r="B89">
-        <v>0.08680304196444934</v>
+        <v>0.1495041526646685</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="1">
-        <v>159</v>
+        <v>88</v>
       </c>
       <c r="B90">
-        <v>0.111213791784838</v>
+        <v>0.01858708081363386</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="1">
-        <v>160</v>
+        <v>89</v>
       </c>
       <c r="B91">
-        <v>0.1832508704416346</v>
+        <v>0.1911984959051655</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="1">
-        <v>162</v>
+        <v>90</v>
       </c>
       <c r="B92">
-        <v>0.03509430534952015</v>
+        <v>0.05311069330699043</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="1">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="B93">
-        <v>0.2074778137709021</v>
+        <v>0.05239522468791943</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="1">
-        <v>164</v>
+        <v>92</v>
       </c>
       <c r="B94">
-        <v>0.2349271852394761</v>
+        <v>0.1699542185823693</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="1">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="B95">
-        <v>0.03319589518050211</v>
+        <v>0.01397287105785879</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="1">
-        <v>171</v>
+        <v>94</v>
       </c>
       <c r="B96">
-        <v>0.2592177752212568</v>
+        <v>0.01397287105785879</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="1">
-        <v>172</v>
+        <v>95</v>
       </c>
       <c r="B97">
-        <v>0.1219767162720542</v>
+        <v>0.05978139638634843</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="1">
-        <v>173</v>
+        <v>96</v>
       </c>
       <c r="B98">
-        <v>0.1340859996334983</v>
+        <v>0.01648193705320629</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="1">
-        <v>176</v>
+        <v>97</v>
       </c>
       <c r="B99">
-        <v>0.0436778449697636</v>
+        <v>0.0635766401259423</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="1">
-        <v>177</v>
+        <v>98</v>
       </c>
       <c r="B100">
-        <v>0.0861143874945758</v>
+        <v>0.001798497342862378</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="1">
-        <v>179</v>
+        <v>99</v>
       </c>
       <c r="B101">
-        <v>0.04090421477002016</v>
+        <v>0.02078115030087662</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="1">
-        <v>180</v>
+        <v>100</v>
       </c>
       <c r="B102">
-        <v>0.1315590537798881</v>
+        <v>0.009816529071650846</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="1">
-        <v>181</v>
+        <v>101</v>
       </c>
       <c r="B103">
-        <v>0.137438152831226</v>
+        <v>0.01484849585742686</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="1">
-        <v>182</v>
+        <v>102</v>
       </c>
       <c r="B104">
-        <v>0.2819126222873713</v>
+        <v>0.01648193705320629</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="1">
-        <v>183</v>
+        <v>103</v>
       </c>
       <c r="B105">
-        <v>0.01648193705320629</v>
+        <v>0.07198787658659651</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="1">
-        <v>184</v>
+        <v>104</v>
       </c>
       <c r="B106">
-        <v>0.08834876164485761</v>
+        <v>0.1990096342797659</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="1">
-        <v>186</v>
+        <v>105</v>
       </c>
       <c r="B107">
-        <v>0.03665017408832692</v>
+        <v>0.02349966132974703</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="1">
-        <v>188</v>
+        <v>106</v>
       </c>
       <c r="B108">
-        <v>0.06269293567894448</v>
+        <v>0.009290504870250576</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="1">
-        <v>189</v>
+        <v>107</v>
       </c>
       <c r="B109">
-        <v>0.08482682792743265</v>
+        <v>0.03078295784073165</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="1">
-        <v>190</v>
+        <v>108</v>
       </c>
       <c r="B110">
-        <v>0.09620670698185817</v>
+        <v>0.04241918636613524</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="1">
-        <v>192</v>
+        <v>109</v>
       </c>
       <c r="B111">
-        <v>0.05298053343828525</v>
+        <v>0.221679423855199</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="1">
-        <v>195</v>
+        <v>110</v>
       </c>
       <c r="B112">
-        <v>0.09786690460257268</v>
+        <v>0.1177983488598102</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="1">
-        <v>196</v>
+        <v>111</v>
       </c>
       <c r="B113">
-        <v>0.3155543883018982</v>
+        <v>0.2212545995968481</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="1">
-        <v>197</v>
+        <v>112</v>
       </c>
       <c r="B114">
-        <v>0.0436778449697636</v>
+        <v>0.252288254468025</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="1">
-        <v>200</v>
+        <v>113</v>
       </c>
       <c r="B115">
-        <v>0.1282756093091442</v>
+        <v>0.00880843248261734</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="1">
-        <v>201</v>
+        <v>114</v>
       </c>
       <c r="B116">
-        <v>0.1472479360747627</v>
+        <v>0.2349271852394761</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="1">
-        <v>204</v>
+        <v>115</v>
       </c>
       <c r="B117">
-        <v>0.01116345346972159</v>
+        <v>0.006952574674729705</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="1">
-        <v>205</v>
+        <v>116</v>
       </c>
       <c r="B118">
-        <v>0.02125750719060754</v>
+        <v>0.01484849585742686</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="1">
-        <v>207</v>
+        <v>117</v>
       </c>
       <c r="B119">
-        <v>0.1086663798689228</v>
+        <v>0.07330034817665385</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="1">
-        <v>208</v>
+        <v>118</v>
       </c>
       <c r="B120">
-        <v>0.02349966132974703</v>
+        <v>0.01369126981724239</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="1">
-        <v>210</v>
+        <v>119</v>
       </c>
       <c r="B121">
-        <v>0.1822863936228697</v>
+        <v>0.05978139638634843</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="1">
-        <v>211</v>
+        <v>120</v>
       </c>
       <c r="B122">
-        <v>0.2061471105046677</v>
+        <v>0.0252288254468025</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="1">
-        <v>212</v>
+        <v>121</v>
       </c>
       <c r="B123">
-        <v>0.1104292129615614</v>
+        <v>0.1001039270046631</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="1">
-        <v>214</v>
+        <v>122</v>
       </c>
       <c r="B124">
-        <v>0.08368982041414696</v>
+        <v>0.02349966098588968</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="1">
-        <v>215</v>
+        <v>123</v>
       </c>
       <c r="B125">
-        <v>0.05239081565540056</v>
+        <v>0.08119540486281507</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="1">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="B126">
-        <v>0.1117830309693971</v>
+        <v>0.03320113428799209</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="1">
-        <v>217</v>
+        <v>125</v>
       </c>
       <c r="B127">
-        <v>0.02154882719442917</v>
+        <v>0.001204890594783496</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="1">
-        <v>219</v>
+        <v>126</v>
       </c>
       <c r="B128">
-        <v>0.03320113428799209</v>
+        <v>0.20183060357442</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="1">
-        <v>220</v>
+        <v>127</v>
       </c>
       <c r="B129">
-        <v>0.2349271852394761</v>
+        <v>0.02349966098588968</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="1">
-        <v>221</v>
+        <v>128</v>
       </c>
       <c r="B130">
-        <v>0.1426575439233851</v>
+        <v>0.191739073395699</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="1">
-        <v>225</v>
+        <v>129</v>
       </c>
       <c r="B131">
-        <v>0.35</v>
+        <v>0.03282010262048745</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="1">
-        <v>230</v>
+        <v>130</v>
       </c>
       <c r="B132">
-        <v>0.08482940268232872</v>
+        <v>0.01115238210569869</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="1">
-        <v>231</v>
+        <v>131</v>
       </c>
       <c r="B133">
-        <v>0.02349966132974703</v>
+        <v>0.2565512186182884</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="1">
-        <v>232</v>
+        <v>132</v>
       </c>
       <c r="B134">
-        <v>0.0436778449697636</v>
+        <v>0.02650462849345728</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="1">
-        <v>233</v>
+        <v>133</v>
       </c>
       <c r="B135">
-        <v>0.1020521971893821</v>
+        <v>0.03665017408832692</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="1">
-        <v>235</v>
+        <v>134</v>
       </c>
       <c r="B136">
-        <v>0.1646431492516703</v>
+        <v>0.1145317940260216</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="1">
-        <v>236</v>
+        <v>135</v>
       </c>
       <c r="B137">
-        <v>0.2462240952593396</v>
+        <v>0.0488405935651084</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="1">
-        <v>237</v>
+        <v>136</v>
       </c>
       <c r="B138">
-        <v>0.01648193705320629</v>
+        <v>0.01538256977098038</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="1">
-        <v>238</v>
+        <v>137</v>
       </c>
       <c r="B139">
-        <v>0.02716659762276537</v>
+        <v>0.04225928168488188</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="1">
-        <v>239</v>
+        <v>138</v>
       </c>
       <c r="B140">
-        <v>0.1407753311451727</v>
+        <v>0.09841250687190764</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="1">
-        <v>240</v>
+        <v>139</v>
       </c>
       <c r="B141">
-        <v>0.1741334246837259</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="1">
-        <v>241</v>
+        <v>140</v>
       </c>
       <c r="B142">
-        <v>0.02349966098588968</v>
+        <v>0.07330034817665385</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="1">
-        <v>242</v>
+        <v>141</v>
       </c>
       <c r="B143">
-        <v>0.35</v>
+        <v>0.01484849585742686</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="1">
-        <v>244</v>
+        <v>142</v>
       </c>
       <c r="B144">
-        <v>0.0232105194110583</v>
+        <v>0.01484849585742686</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="1">
-        <v>248</v>
+        <v>143</v>
       </c>
       <c r="B145">
-        <v>0.02454132267912712</v>
+        <v>0.01516605640577604</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="1">
-        <v>249</v>
+        <v>144</v>
       </c>
       <c r="B146">
-        <v>0.07151253435953821</v>
+        <v>0.09559924795258276</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="1">
-        <v>251</v>
+        <v>145</v>
       </c>
       <c r="B147">
-        <v>0.0991132471516656</v>
+        <v>0.02125750412314458</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="1">
-        <v>252</v>
+        <v>146</v>
       </c>
       <c r="B148">
-        <v>0.3</v>
+        <v>0.2464336169444356</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="1">
-        <v>254</v>
+        <v>147</v>
       </c>
       <c r="B149">
-        <v>0.04154722071741925</v>
+        <v>0.01484848818031886</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="1">
-        <v>256</v>
+        <v>148</v>
       </c>
       <c r="B150">
-        <v>0.04241231385406748</v>
+        <v>0.01241445914444007</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="1">
-        <v>257</v>
+        <v>149</v>
       </c>
       <c r="B151">
-        <v>0.35</v>
+        <v>0.02655534665349521</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="1">
-        <v>258</v>
+        <v>150</v>
       </c>
       <c r="B152">
-        <v>0.1081235405124479</v>
+        <v>0.1301211986021265</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="1">
-        <v>259</v>
+        <v>151</v>
       </c>
       <c r="B153">
-        <v>0.03206890232728606</v>
+        <v>0.007682462891698736</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="1">
-        <v>260</v>
+        <v>152</v>
       </c>
       <c r="B154">
-        <v>0.0436778449697636</v>
+        <v>0.2804054242257651</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" s="1">
-        <v>261</v>
+        <v>153</v>
       </c>
       <c r="B155">
-        <v>0.050457650893605</v>
+        <v>0.06818636613523914</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="1">
-        <v>263</v>
+        <v>154</v>
       </c>
       <c r="B156">
-        <v>0.04908264535825423</v>
+        <v>0.08680304196444934</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="1">
-        <v>264</v>
+        <v>155</v>
       </c>
       <c r="B157">
-        <v>0.08495074065711845</v>
+        <v>0.01397287105785879</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="1">
-        <v>265</v>
+        <v>156</v>
       </c>
       <c r="B158">
-        <v>0.0333020495897793</v>
+        <v>0.02349966132974703</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="1">
-        <v>270</v>
+        <v>157</v>
       </c>
       <c r="B159">
-        <v>0.05955653289353125</v>
+        <v>0.01484849585742686</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="1">
-        <v>271</v>
+        <v>158</v>
       </c>
       <c r="B160">
-        <v>0.05938686091258934</v>
+        <v>0.03078295784073165</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="1">
-        <v>272</v>
+        <v>159</v>
       </c>
       <c r="B161">
-        <v>0.25</v>
+        <v>0.111213791784838</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="1">
-        <v>273</v>
+        <v>160</v>
       </c>
       <c r="B162">
-        <v>0.04248855464559233</v>
+        <v>0.1832508704416346</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="1">
-        <v>275</v>
+        <v>161</v>
       </c>
       <c r="B163">
-        <v>0.1327767332674761</v>
+        <v>0.06576166045271555</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="1">
-        <v>277</v>
+        <v>162</v>
       </c>
       <c r="B164">
-        <v>0.1487099412595732</v>
+        <v>0.03509430534952015</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="1">
-        <v>278</v>
+        <v>163</v>
       </c>
       <c r="B165">
-        <v>0.01610892420657904</v>
+        <v>0.2074778137709021</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="1">
-        <v>279</v>
+        <v>164</v>
       </c>
       <c r="B166">
-        <v>0.09902129205155639</v>
+        <v>0.2349271852394761</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" s="1">
-        <v>280</v>
+        <v>165</v>
       </c>
       <c r="B167">
-        <v>0.08979292651640096</v>
+        <v>0.03319589518050211</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="1">
-        <v>281</v>
+        <v>166</v>
       </c>
       <c r="B168">
-        <v>0.01484849585742686</v>
+        <v>0.02033655184134774</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="1">
-        <v>282</v>
+        <v>167</v>
       </c>
       <c r="B169">
-        <v>0.0436778449697636</v>
+        <v>0.1168435252753789</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="1">
-        <v>283</v>
+        <v>168</v>
       </c>
       <c r="B170">
-        <v>0.08073224142976801</v>
+        <v>0.01484848818031886</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="1">
-        <v>285</v>
+        <v>169</v>
       </c>
       <c r="B171">
-        <v>0.02349966098588968</v>
+        <v>0.0436778449697636</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" s="1">
-        <v>286</v>
+        <v>170</v>
       </c>
       <c r="B172">
-        <v>0.000766844056382312</v>
+        <v>0.008230804471321239</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="1">
-        <v>287</v>
+        <v>171</v>
       </c>
       <c r="B173">
-        <v>0.05311069330699043</v>
+        <v>0.2592177752212568</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="1">
-        <v>288</v>
+        <v>172</v>
       </c>
       <c r="B174">
-        <v>0.1177983488598102</v>
+        <v>0.1219767162720542</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="1">
-        <v>289</v>
+        <v>173</v>
       </c>
       <c r="B175">
-        <v>0.01995128275609309</v>
+        <v>0.1340859996334983</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="1">
-        <v>291</v>
+        <v>174</v>
       </c>
       <c r="B176">
-        <v>0.1167580914141253</v>
+        <v>0.01591757238150021</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" s="1">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="B177">
-        <v>0.01992228512609367</v>
+        <v>0.01324625351942115</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="1">
-        <v>293</v>
+        <v>176</v>
       </c>
       <c r="B178">
-        <v>0.01725185286986227</v>
+        <v>0.0436778449697636</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" s="1">
-        <v>294</v>
+        <v>177</v>
       </c>
       <c r="B179">
-        <v>0.01591666666666667</v>
+        <v>0.0861143874945758</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" s="1">
-        <v>295</v>
+        <v>178</v>
       </c>
       <c r="B180">
-        <v>0.07411839838739234</v>
+        <v>0.01648193705320629</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="1">
-        <v>296</v>
+        <v>179</v>
       </c>
       <c r="B181">
-        <v>0.02655534665349521</v>
+        <v>0.04090421477002016</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" s="1">
-        <v>297</v>
+        <v>180</v>
       </c>
       <c r="B182">
-        <v>0.1805763572437675</v>
+        <v>0.1315590537798881</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="1">
-        <v>298</v>
+        <v>181</v>
       </c>
       <c r="B183">
-        <v>0.1099505222649808</v>
+        <v>0.137438152831226</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" s="1">
-        <v>300</v>
+        <v>182</v>
       </c>
       <c r="B184">
-        <v>0.3</v>
+        <v>0.2819126222873713</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="1">
-        <v>301</v>
+        <v>183</v>
       </c>
       <c r="B185">
-        <v>0.2819126222873713</v>
+        <v>0.01648193705320629</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="1">
-        <v>302</v>
+        <v>184</v>
       </c>
       <c r="B186">
-        <v>0.0982547826179323</v>
+        <v>0.08834876164485761</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="1">
-        <v>303</v>
+        <v>185</v>
       </c>
       <c r="B187">
-        <v>0.161464482859536</v>
+        <v>0.01484849585742686</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" s="1">
-        <v>306</v>
+        <v>186</v>
       </c>
       <c r="B188">
-        <v>0.09547989760258332</v>
+        <v>0.03665017408832692</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" s="1">
-        <v>307</v>
+        <v>187</v>
       </c>
       <c r="B189">
-        <v>0.0436778449697636</v>
+        <v>0.07701050529513613</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" s="1">
-        <v>308</v>
+        <v>188</v>
       </c>
       <c r="B190">
-        <v>0.07853223257320678</v>
+        <v>0.06269293567894448</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" s="1">
-        <v>309</v>
+        <v>189</v>
       </c>
       <c r="B191">
-        <v>0.03319950132032316</v>
+        <v>0.08482682792743265</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" s="1">
-        <v>310</v>
+        <v>190</v>
       </c>
       <c r="B192">
-        <v>0.1593320799209713</v>
+        <v>0.09620670698185817</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" s="1">
-        <v>311</v>
+        <v>191</v>
       </c>
       <c r="B193">
-        <v>0.0615496372792508</v>
+        <v>0.02340057147105998</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" s="1">
-        <v>315</v>
+        <v>192</v>
       </c>
       <c r="B194">
-        <v>0.08482462770813495</v>
+        <v>0.05298053343828525</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" s="1">
-        <v>318</v>
+        <v>193</v>
       </c>
       <c r="B195">
-        <v>0.1693610146266849</v>
+        <v>0.02349966193373901</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" s="1">
-        <v>320</v>
+        <v>194</v>
       </c>
       <c r="B196">
-        <v>0.02349966132974703</v>
+        <v>0.01116345346972159</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" s="1">
-        <v>321</v>
+        <v>195</v>
       </c>
       <c r="B197">
-        <v>0.05138266254527687</v>
+        <v>0.09786690460257268</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" s="1">
-        <v>322</v>
+        <v>196</v>
       </c>
       <c r="B198">
-        <v>0.02944958721495254</v>
+        <v>0.3155543883018982</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" s="1">
-        <v>323</v>
+        <v>197</v>
       </c>
       <c r="B199">
-        <v>0.2024535436408223</v>
+        <v>0.0436778449697636</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" s="1">
-        <v>324</v>
+        <v>198</v>
       </c>
       <c r="B200">
-        <v>0.1070425660742938</v>
+        <v>0.020540663368151</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" s="1">
-        <v>325</v>
+        <v>199</v>
       </c>
       <c r="B201">
-        <v>0.1963305814330169</v>
+        <v>0.04581271761040865</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" s="1">
-        <v>326</v>
+        <v>200</v>
       </c>
       <c r="B202">
-        <v>0.2843548011728056</v>
+        <v>0.1282756093091442</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" s="1">
-        <v>327</v>
+        <v>201</v>
       </c>
       <c r="B203">
-        <v>0.002998889931680341</v>
+        <v>0.1472479360747627</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" s="1">
-        <v>328</v>
+        <v>202</v>
       </c>
       <c r="B204">
-        <v>0.1131178211471505</v>
+        <v>0.01006677565519259</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" s="1">
-        <v>329</v>
+        <v>203</v>
       </c>
       <c r="B205">
-        <v>0.03151914971596115</v>
+        <v>0.06054918107232599</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" s="1">
-        <v>330</v>
+        <v>204</v>
       </c>
       <c r="B206">
-        <v>0.2819126222873713</v>
+        <v>0.01116345346972159</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" s="1">
-        <v>331</v>
+        <v>205</v>
       </c>
       <c r="B207">
-        <v>0.06054918107232599</v>
+        <v>0.02125750719060754</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="1">
-        <v>332</v>
+        <v>206</v>
       </c>
       <c r="B208">
-        <v>0.01648193705320629</v>
+        <v>0.04367614261350448</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" s="1">
-        <v>333</v>
+        <v>207</v>
       </c>
       <c r="B209">
-        <v>0.04241231385406748</v>
+        <v>0.1086663798689228</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" s="1">
-        <v>334</v>
+        <v>208</v>
       </c>
       <c r="B210">
-        <v>0.02529301814183617</v>
+        <v>0.02349966132974703</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" s="1">
-        <v>337</v>
+        <v>209</v>
       </c>
       <c r="B211">
-        <v>0.1408172121138728</v>
+        <v>0.04225928168488188</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" s="1">
-        <v>338</v>
+        <v>210</v>
       </c>
       <c r="B212">
-        <v>0.141281422502094</v>
+        <v>0.1822863936228697</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" s="1">
-        <v>339</v>
+        <v>211</v>
       </c>
       <c r="B213">
-        <v>0.09559924795258276</v>
+        <v>0.2061471105046677</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" s="1">
-        <v>341</v>
+        <v>212</v>
       </c>
       <c r="B214">
-        <v>0.01334677478468023</v>
+        <v>0.1104292129615614</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" s="1">
-        <v>343</v>
+        <v>213</v>
       </c>
       <c r="B215">
-        <v>0.2247985157408044</v>
+        <v>0.06467812795428232</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" s="1">
-        <v>346</v>
+        <v>214</v>
       </c>
       <c r="B216">
-        <v>0.0638074389657305</v>
+        <v>0.08368982041414696</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" s="1">
-        <v>347</v>
+        <v>215</v>
       </c>
       <c r="B217">
-        <v>0.06373283196838851</v>
+        <v>0.05239081565540056</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" s="1">
-        <v>349</v>
+        <v>216</v>
       </c>
       <c r="B218">
-        <v>0.04248855464559233</v>
+        <v>0.1117830309693971</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219" s="1">
-        <v>350</v>
+        <v>217</v>
       </c>
       <c r="B219">
-        <v>0.2349271852394761</v>
+        <v>0.02154882719442917</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" s="1">
-        <v>352</v>
+        <v>218</v>
       </c>
       <c r="B220">
-        <v>0.1181968114348543</v>
+        <v>0.02349966132974703</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" s="1">
-        <v>353</v>
+        <v>219</v>
       </c>
       <c r="B221">
-        <v>0.1221672530694521</v>
+        <v>0.03320113428799209</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" s="1">
-        <v>354</v>
+        <v>220</v>
       </c>
       <c r="B222">
-        <v>0.1194140828314373</v>
+        <v>0.2349271852394761</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223" s="1">
-        <v>355</v>
+        <v>221</v>
       </c>
       <c r="B223">
-        <v>0.1483459409932197</v>
+        <v>0.1426575439233851</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" s="1">
-        <v>356</v>
+        <v>222</v>
       </c>
       <c r="B224">
-        <v>0.1790832248493839</v>
+        <v>0.01591666748471076</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" s="1">
-        <v>357</v>
+        <v>223</v>
       </c>
       <c r="B225">
-        <v>0.03078295784073165</v>
+        <v>0.02784585853032802</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" s="1">
-        <v>358</v>
+        <v>224</v>
       </c>
       <c r="B226">
-        <v>0.01484849585742686</v>
+        <v>0.01648193705320629</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" s="1">
-        <v>359</v>
+        <v>225</v>
       </c>
       <c r="B227">
-        <v>0.2908374564779183</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" s="1">
-        <v>361</v>
+        <v>226</v>
       </c>
       <c r="B228">
-        <v>0.0436778449697636</v>
+        <v>0.01484849585742686</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" s="1">
-        <v>362</v>
+        <v>227</v>
       </c>
       <c r="B229">
-        <v>0.09344009163109404</v>
+        <v>0.04365915338097856</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" s="1">
-        <v>363</v>
+        <v>228</v>
       </c>
       <c r="B230">
-        <v>0.01906784203241418</v>
+        <v>0.007913374304945859</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" s="1">
-        <v>364</v>
+        <v>229</v>
       </c>
       <c r="B231">
-        <v>0.1805763572437675</v>
+        <v>0.06076286922386041</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" s="1">
-        <v>367</v>
+        <v>230</v>
       </c>
       <c r="B232">
-        <v>0.01484849585742686</v>
+        <v>0.08482940268232872</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" s="1">
-        <v>368</v>
+        <v>231</v>
       </c>
       <c r="B233">
-        <v>0.01484849585742686</v>
+        <v>0.02349966132974703</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" s="1">
-        <v>371</v>
+        <v>232</v>
       </c>
       <c r="B234">
-        <v>0.06373283196838851</v>
+        <v>0.0436778449697636</v>
       </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235" s="1">
-        <v>373</v>
+        <v>233</v>
       </c>
       <c r="B235">
-        <v>0.3</v>
+        <v>0.1020521971893821</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" s="1">
-        <v>374</v>
+        <v>234</v>
       </c>
       <c r="B236">
-        <v>0.06704299981674912</v>
+        <v>0.02125750412314458</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" s="1">
-        <v>375</v>
+        <v>235</v>
       </c>
       <c r="B237">
-        <v>0.01858708081363386</v>
+        <v>0.1646431492516703</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" s="1">
-        <v>376</v>
+        <v>236</v>
       </c>
       <c r="B238">
-        <v>0.08497710929118467</v>
+        <v>0.2462240952593396</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" s="1">
-        <v>377</v>
+        <v>237</v>
       </c>
       <c r="B239">
-        <v>0.06040940816146227</v>
+        <v>0.01648193705320629</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" s="1">
-        <v>378</v>
+        <v>238</v>
       </c>
       <c r="B240">
-        <v>0.02349966098588968</v>
+        <v>0.02716659762276537</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" s="1">
-        <v>379</v>
+        <v>239</v>
       </c>
       <c r="B241">
-        <v>0.2819126222873713</v>
+        <v>0.1407753311451727</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" s="1">
-        <v>380</v>
+        <v>240</v>
       </c>
       <c r="B242">
-        <v>0.02349966098588968</v>
+        <v>0.1741334246837259</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" s="1">
-        <v>381</v>
+        <v>241</v>
       </c>
       <c r="B243">
-        <v>0.05523512103927005</v>
+        <v>0.02349966098588968</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244" s="1">
-        <v>382</v>
+        <v>242</v>
       </c>
       <c r="B244">
-        <v>0.03435785175077796</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" s="1">
-        <v>384</v>
+        <v>243</v>
       </c>
       <c r="B245">
-        <v>0.2655534665349521</v>
+        <v>0.02748763056624519</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" s="1">
-        <v>386</v>
+        <v>244</v>
       </c>
       <c r="B246">
-        <v>0.08482462770813495</v>
+        <v>0.0232105194110583</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" s="1">
-        <v>387</v>
+        <v>245</v>
       </c>
       <c r="B247">
-        <v>0.124203445248403</v>
+        <v>0.03320113428799209</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" s="1">
-        <v>388</v>
+        <v>246</v>
       </c>
       <c r="B248">
-        <v>0.2896642951570746</v>
+        <v>0.02290635880520433</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" s="1">
-        <v>390</v>
+        <v>247</v>
       </c>
       <c r="B249">
-        <v>0.03665017408832692</v>
+        <v>0.01725185431867034</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" s="1">
-        <v>391</v>
+        <v>248</v>
       </c>
       <c r="B250">
-        <v>0.01648193705320629</v>
+        <v>0.02454132267912712</v>
       </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251" s="1">
-        <v>392</v>
+        <v>249</v>
       </c>
       <c r="B251">
-        <v>0.3</v>
+        <v>0.07151253435953821</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" s="1">
+        <v>250</v>
+      </c>
+      <c r="B252">
+        <v>0.0272471314825467</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2">
+      <c r="A253" s="1">
+        <v>251</v>
+      </c>
+      <c r="B253">
+        <v>0.0991132471516656</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2">
+      <c r="A254" s="1">
+        <v>252</v>
+      </c>
+      <c r="B254">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2">
+      <c r="A255" s="1">
+        <v>253</v>
+      </c>
+      <c r="B255">
+        <v>0.01484848818031886</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="A256" s="1">
+        <v>254</v>
+      </c>
+      <c r="B256">
+        <v>0.04154722071741925</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="A257" s="1">
+        <v>255</v>
+      </c>
+      <c r="B257">
+        <v>0.04248855464559233</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
+      <c r="A258" s="1">
+        <v>256</v>
+      </c>
+      <c r="B258">
+        <v>0.04241231385406748</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="A259" s="1">
+        <v>257</v>
+      </c>
+      <c r="B259">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
+      <c r="A260" s="1">
+        <v>258</v>
+      </c>
+      <c r="B260">
+        <v>0.1081235405124479</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2">
+      <c r="A261" s="1">
+        <v>259</v>
+      </c>
+      <c r="B261">
+        <v>0.03206890232728606</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2">
+      <c r="A262" s="1">
+        <v>260</v>
+      </c>
+      <c r="B262">
+        <v>0.0436778449697636</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2">
+      <c r="A263" s="1">
+        <v>261</v>
+      </c>
+      <c r="B263">
+        <v>0.050457650893605</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2">
+      <c r="A264" s="1">
+        <v>262</v>
+      </c>
+      <c r="B264">
+        <v>0.002251108667766172</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2">
+      <c r="A265" s="1">
+        <v>263</v>
+      </c>
+      <c r="B265">
+        <v>0.04908264535825423</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2">
+      <c r="A266" s="1">
+        <v>264</v>
+      </c>
+      <c r="B266">
+        <v>0.08495074065711845</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2">
+      <c r="A267" s="1">
+        <v>265</v>
+      </c>
+      <c r="B267">
+        <v>0.0333020495897793</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2">
+      <c r="A268" s="1">
+        <v>266</v>
+      </c>
+      <c r="B268">
+        <v>0.02110553750404932</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2">
+      <c r="A269" s="1">
+        <v>267</v>
+      </c>
+      <c r="B269">
+        <v>0.004442475808079199</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2">
+      <c r="A270" s="1">
+        <v>268</v>
+      </c>
+      <c r="B270">
+        <v>0.01858708081363386</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2">
+      <c r="A271" s="1">
+        <v>269</v>
+      </c>
+      <c r="B271">
+        <v>0.1327767332674761</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2">
+      <c r="A272" s="1">
+        <v>270</v>
+      </c>
+      <c r="B272">
+        <v>0.05955653289353125</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2">
+      <c r="A273" s="1">
+        <v>271</v>
+      </c>
+      <c r="B273">
+        <v>0.05938686091258934</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2">
+      <c r="A274" s="1">
+        <v>272</v>
+      </c>
+      <c r="B274">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2">
+      <c r="A275" s="1">
+        <v>273</v>
+      </c>
+      <c r="B275">
+        <v>0.04248855464559233</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2">
+      <c r="A276" s="1">
+        <v>274</v>
+      </c>
+      <c r="B276">
+        <v>0.01648193705320629</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2">
+      <c r="A277" s="1">
+        <v>275</v>
+      </c>
+      <c r="B277">
+        <v>0.1327767332674761</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2">
+      <c r="A278" s="1">
+        <v>276</v>
+      </c>
+      <c r="B278">
+        <v>0.01078886374982739</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2">
+      <c r="A279" s="1">
+        <v>277</v>
+      </c>
+      <c r="B279">
+        <v>0.1487099412595732</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2">
+      <c r="A280" s="1">
+        <v>278</v>
+      </c>
+      <c r="B280">
+        <v>0.01610892420657904</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2">
+      <c r="A281" s="1">
+        <v>279</v>
+      </c>
+      <c r="B281">
+        <v>0.09902129205155639</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2">
+      <c r="A282" s="1">
+        <v>280</v>
+      </c>
+      <c r="B282">
+        <v>0.08979292651640096</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2">
+      <c r="A283" s="1">
+        <v>281</v>
+      </c>
+      <c r="B283">
+        <v>0.01484849585742686</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2">
+      <c r="A284" s="1">
+        <v>282</v>
+      </c>
+      <c r="B284">
+        <v>0.0436778449697636</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2">
+      <c r="A285" s="1">
+        <v>283</v>
+      </c>
+      <c r="B285">
+        <v>0.08073224142976801</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2">
+      <c r="A286" s="1">
+        <v>284</v>
+      </c>
+      <c r="B286">
+        <v>0.01484849585742686</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2">
+      <c r="A287" s="1">
+        <v>285</v>
+      </c>
+      <c r="B287">
+        <v>0.02349966098588968</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2">
+      <c r="A288" s="1">
+        <v>286</v>
+      </c>
+      <c r="B288">
+        <v>0.000766844056382312</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2">
+      <c r="A289" s="1">
+        <v>287</v>
+      </c>
+      <c r="B289">
+        <v>0.05311069330699043</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2">
+      <c r="A290" s="1">
+        <v>288</v>
+      </c>
+      <c r="B290">
+        <v>0.1177983488598102</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2">
+      <c r="A291" s="1">
+        <v>289</v>
+      </c>
+      <c r="B291">
+        <v>0.01995128275609309</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2">
+      <c r="A292" s="1">
+        <v>290</v>
+      </c>
+      <c r="B292">
+        <v>0.01591666666666667</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2">
+      <c r="A293" s="1">
+        <v>291</v>
+      </c>
+      <c r="B293">
+        <v>0.1167580914141253</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2">
+      <c r="A294" s="1">
+        <v>292</v>
+      </c>
+      <c r="B294">
+        <v>0.01992228512609367</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2">
+      <c r="A295" s="1">
+        <v>293</v>
+      </c>
+      <c r="B295">
+        <v>0.01725185286986227</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2">
+      <c r="A296" s="1">
+        <v>294</v>
+      </c>
+      <c r="B296">
+        <v>0.01591666666666667</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2">
+      <c r="A297" s="1">
+        <v>295</v>
+      </c>
+      <c r="B297">
+        <v>0.07411839838739234</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2">
+      <c r="A298" s="1">
+        <v>296</v>
+      </c>
+      <c r="B298">
+        <v>0.02655534665349521</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2">
+      <c r="A299" s="1">
+        <v>297</v>
+      </c>
+      <c r="B299">
+        <v>0.1805763572437675</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2">
+      <c r="A300" s="1">
+        <v>298</v>
+      </c>
+      <c r="B300">
+        <v>0.1099505222649808</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2">
+      <c r="A301" s="1">
+        <v>299</v>
+      </c>
+      <c r="B301">
+        <v>0.01678172947609184</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2">
+      <c r="A302" s="1">
+        <v>300</v>
+      </c>
+      <c r="B302">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2">
+      <c r="A303" s="1">
+        <v>301</v>
+      </c>
+      <c r="B303">
+        <v>0.2819126222873713</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2">
+      <c r="A304" s="1">
+        <v>302</v>
+      </c>
+      <c r="B304">
+        <v>0.0982547826179323</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2">
+      <c r="A305" s="1">
+        <v>303</v>
+      </c>
+      <c r="B305">
+        <v>0.161464482859536</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2">
+      <c r="A306" s="1">
+        <v>304</v>
+      </c>
+      <c r="B306">
+        <v>0.07762715832601698</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2">
+      <c r="A307" s="1">
+        <v>305</v>
+      </c>
+      <c r="B307">
+        <v>0.0524759569293492</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2">
+      <c r="A308" s="1">
+        <v>306</v>
+      </c>
+      <c r="B308">
+        <v>0.09547989760258332</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2">
+      <c r="A309" s="1">
+        <v>307</v>
+      </c>
+      <c r="B309">
+        <v>0.0436778449697636</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2">
+      <c r="A310" s="1">
+        <v>308</v>
+      </c>
+      <c r="B310">
+        <v>0.07853223257320678</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2">
+      <c r="A311" s="1">
+        <v>309</v>
+      </c>
+      <c r="B311">
+        <v>0.03319950132032316</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2">
+      <c r="A312" s="1">
+        <v>310</v>
+      </c>
+      <c r="B312">
+        <v>0.1593320799209713</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2">
+      <c r="A313" s="1">
+        <v>311</v>
+      </c>
+      <c r="B313">
+        <v>0.0615496372792508</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2">
+      <c r="A314" s="1">
+        <v>312</v>
+      </c>
+      <c r="B314">
+        <v>0.06576166045271555</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2">
+      <c r="A315" s="1">
+        <v>313</v>
+      </c>
+      <c r="B315">
+        <v>0.0151372952680815</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2">
+      <c r="A316" s="1">
+        <v>314</v>
+      </c>
+      <c r="B316">
+        <v>0.01324626168224299</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2">
+      <c r="A317" s="1">
+        <v>315</v>
+      </c>
+      <c r="B317">
+        <v>0.08482462770813495</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2">
+      <c r="A318" s="1">
+        <v>316</v>
+      </c>
+      <c r="B318">
+        <v>0.04908264535825423</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2">
+      <c r="A319" s="1">
+        <v>317</v>
+      </c>
+      <c r="B319">
+        <v>0.0371774853148933</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2">
+      <c r="A320" s="1">
+        <v>318</v>
+      </c>
+      <c r="B320">
+        <v>0.1693610146266849</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2">
+      <c r="A321" s="1">
+        <v>319</v>
+      </c>
+      <c r="B321">
+        <v>0.01484849585742686</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2">
+      <c r="A322" s="1">
+        <v>320</v>
+      </c>
+      <c r="B322">
+        <v>0.02349966132974703</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2">
+      <c r="A323" s="1">
+        <v>321</v>
+      </c>
+      <c r="B323">
+        <v>0.05138266254527687</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2">
+      <c r="A324" s="1">
+        <v>322</v>
+      </c>
+      <c r="B324">
+        <v>0.02944958721495254</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2">
+      <c r="A325" s="1">
+        <v>323</v>
+      </c>
+      <c r="B325">
+        <v>0.2024535436408223</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2">
+      <c r="A326" s="1">
+        <v>324</v>
+      </c>
+      <c r="B326">
+        <v>0.1070425660742938</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2">
+      <c r="A327" s="1">
+        <v>325</v>
+      </c>
+      <c r="B327">
+        <v>0.1963305814330169</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2">
+      <c r="A328" s="1">
+        <v>326</v>
+      </c>
+      <c r="B328">
+        <v>0.2843548011728056</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2">
+      <c r="A329" s="1">
+        <v>327</v>
+      </c>
+      <c r="B329">
+        <v>0.002998889931680341</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2">
+      <c r="A330" s="1">
+        <v>328</v>
+      </c>
+      <c r="B330">
+        <v>0.1131178211471505</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2">
+      <c r="A331" s="1">
+        <v>329</v>
+      </c>
+      <c r="B331">
+        <v>0.03151914971596115</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2">
+      <c r="A332" s="1">
+        <v>330</v>
+      </c>
+      <c r="B332">
+        <v>0.2819126222873713</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2">
+      <c r="A333" s="1">
+        <v>331</v>
+      </c>
+      <c r="B333">
+        <v>0.06054918107232599</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2">
+      <c r="A334" s="1">
+        <v>332</v>
+      </c>
+      <c r="B334">
+        <v>0.01648193705320629</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2">
+      <c r="A335" s="1">
+        <v>333</v>
+      </c>
+      <c r="B335">
+        <v>0.04241231385406748</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2">
+      <c r="A336" s="1">
+        <v>334</v>
+      </c>
+      <c r="B336">
+        <v>0.02529301814183617</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2">
+      <c r="A337" s="1">
+        <v>335</v>
+      </c>
+      <c r="B337">
+        <v>0.02349966132974703</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2">
+      <c r="A338" s="1">
+        <v>336</v>
+      </c>
+      <c r="B338">
+        <v>0.01484849585742686</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2">
+      <c r="A339" s="1">
+        <v>337</v>
+      </c>
+      <c r="B339">
+        <v>0.1408172121138728</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2">
+      <c r="A340" s="1">
+        <v>338</v>
+      </c>
+      <c r="B340">
+        <v>0.141281422502094</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2">
+      <c r="A341" s="1">
+        <v>339</v>
+      </c>
+      <c r="B341">
+        <v>0.09559924795258276</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2">
+      <c r="A342" s="1">
+        <v>340</v>
+      </c>
+      <c r="B342">
+        <v>0.01041427402993319</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2">
+      <c r="A343" s="1">
+        <v>341</v>
+      </c>
+      <c r="B343">
+        <v>0.01334677478468023</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2">
+      <c r="A344" s="1">
+        <v>342</v>
+      </c>
+      <c r="B344">
+        <v>0.04777884368700752</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2">
+      <c r="A345" s="1">
+        <v>343</v>
+      </c>
+      <c r="B345">
+        <v>0.2247985157408044</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2">
+      <c r="A346" s="1">
+        <v>344</v>
+      </c>
+      <c r="B346">
+        <v>0.01487099412595732</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2">
+      <c r="A347" s="1">
+        <v>345</v>
+      </c>
+      <c r="B347">
+        <v>0.002655332600329852</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2">
+      <c r="A348" s="1">
+        <v>346</v>
+      </c>
+      <c r="B348">
+        <v>0.0638074389657305</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2">
+      <c r="A349" s="1">
+        <v>347</v>
+      </c>
+      <c r="B349">
+        <v>0.06373283196838851</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2">
+      <c r="A350" s="1">
+        <v>348</v>
+      </c>
+      <c r="B350">
+        <v>0.05039398937144952</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2">
+      <c r="A351" s="1">
+        <v>349</v>
+      </c>
+      <c r="B351">
+        <v>0.04248855464559233</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2">
+      <c r="A352" s="1">
+        <v>350</v>
+      </c>
+      <c r="B352">
+        <v>0.2349271852394761</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2">
+      <c r="A353" s="1">
+        <v>351</v>
+      </c>
+      <c r="B353">
+        <v>0.1177983488598102</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2">
+      <c r="A354" s="1">
+        <v>352</v>
+      </c>
+      <c r="B354">
+        <v>0.1181968114348543</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2">
+      <c r="A355" s="1">
+        <v>353</v>
+      </c>
+      <c r="B355">
+        <v>0.1221672530694521</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2">
+      <c r="A356" s="1">
+        <v>354</v>
+      </c>
+      <c r="B356">
+        <v>0.1194140828314373</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2">
+      <c r="A357" s="1">
+        <v>355</v>
+      </c>
+      <c r="B357">
+        <v>0.1483459409932197</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2">
+      <c r="A358" s="1">
+        <v>356</v>
+      </c>
+      <c r="B358">
+        <v>0.1790832248493839</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2">
+      <c r="A359" s="1">
+        <v>357</v>
+      </c>
+      <c r="B359">
+        <v>0.03078295784073165</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2">
+      <c r="A360" s="1">
+        <v>358</v>
+      </c>
+      <c r="B360">
+        <v>0.01484849585742686</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2">
+      <c r="A361" s="1">
+        <v>359</v>
+      </c>
+      <c r="B361">
+        <v>0.2908374564779183</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2">
+      <c r="A362" s="1">
+        <v>360</v>
+      </c>
+      <c r="B362">
+        <v>0.02349966098588968</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2">
+      <c r="A363" s="1">
+        <v>361</v>
+      </c>
+      <c r="B363">
+        <v>0.0436778449697636</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2">
+      <c r="A364" s="1">
+        <v>362</v>
+      </c>
+      <c r="B364">
+        <v>0.09344009163109404</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2">
+      <c r="A365" s="1">
+        <v>363</v>
+      </c>
+      <c r="B365">
+        <v>0.01906784203241418</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2">
+      <c r="A366" s="1">
+        <v>364</v>
+      </c>
+      <c r="B366">
+        <v>0.1805763572437675</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2">
+      <c r="A367" s="1">
+        <v>365</v>
+      </c>
+      <c r="B367">
+        <v>0.01490935066866363</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2">
+      <c r="A368" s="1">
+        <v>366</v>
+      </c>
+      <c r="B368">
+        <v>0.015382572842221</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2">
+      <c r="A369" s="1">
+        <v>367</v>
+      </c>
+      <c r="B369">
+        <v>0.01484849585742686</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2">
+      <c r="A370" s="1">
+        <v>368</v>
+      </c>
+      <c r="B370">
+        <v>0.01484849585742686</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2">
+      <c r="A371" s="1">
+        <v>369</v>
+      </c>
+      <c r="B371">
+        <v>0.001798497342862378</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2">
+      <c r="A372" s="1">
+        <v>370</v>
+      </c>
+      <c r="B372">
+        <v>0.01538256990907531</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2">
+      <c r="A373" s="1">
+        <v>371</v>
+      </c>
+      <c r="B373">
+        <v>0.06373283196838851</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2">
+      <c r="A374" s="1">
+        <v>372</v>
+      </c>
+      <c r="B374">
+        <v>0.05311069330699043</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2">
+      <c r="A375" s="1">
+        <v>373</v>
+      </c>
+      <c r="B375">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2">
+      <c r="A376" s="1">
+        <v>374</v>
+      </c>
+      <c r="B376">
+        <v>0.06704299981674912</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2">
+      <c r="A377" s="1">
+        <v>375</v>
+      </c>
+      <c r="B377">
+        <v>0.01858708081363386</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2">
+      <c r="A378" s="1">
+        <v>376</v>
+      </c>
+      <c r="B378">
+        <v>0.08497710929118467</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2">
+      <c r="A379" s="1">
+        <v>377</v>
+      </c>
+      <c r="B379">
+        <v>0.06040940816146227</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2">
+      <c r="A380" s="1">
+        <v>378</v>
+      </c>
+      <c r="B380">
+        <v>0.02349966098588968</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2">
+      <c r="A381" s="1">
+        <v>379</v>
+      </c>
+      <c r="B381">
+        <v>0.2819126222873713</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2">
+      <c r="A382" s="1">
+        <v>380</v>
+      </c>
+      <c r="B382">
+        <v>0.02349966098588968</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2">
+      <c r="A383" s="1">
+        <v>381</v>
+      </c>
+      <c r="B383">
+        <v>0.05523512103927005</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2">
+      <c r="A384" s="1">
+        <v>382</v>
+      </c>
+      <c r="B384">
+        <v>0.03435785175077796</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2">
+      <c r="A385" s="1">
+        <v>383</v>
+      </c>
+      <c r="B385">
+        <v>0.0371774853148933</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2">
+      <c r="A386" s="1">
+        <v>384</v>
+      </c>
+      <c r="B386">
+        <v>0.2655534665349521</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2">
+      <c r="A387" s="1">
+        <v>385</v>
+      </c>
+      <c r="B387">
+        <v>0.02365915338097856</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2">
+      <c r="A388" s="1">
+        <v>386</v>
+      </c>
+      <c r="B388">
+        <v>0.08482462770813495</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2">
+      <c r="A389" s="1">
+        <v>387</v>
+      </c>
+      <c r="B389">
+        <v>0.124203445248403</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2">
+      <c r="A390" s="1">
+        <v>388</v>
+      </c>
+      <c r="B390">
+        <v>0.2896642951570746</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2">
+      <c r="A391" s="1">
+        <v>389</v>
+      </c>
+      <c r="B391">
+        <v>0.01591666666666667</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2">
+      <c r="A392" s="1">
+        <v>390</v>
+      </c>
+      <c r="B392">
+        <v>0.03665017408832692</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2">
+      <c r="A393" s="1">
+        <v>391</v>
+      </c>
+      <c r="B393">
+        <v>0.01648193705320629</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2">
+      <c r="A394" s="1">
+        <v>392</v>
+      </c>
+      <c r="B394">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2">
+      <c r="A395" s="1">
         <v>393</v>
       </c>
-      <c r="B252">
+      <c r="B395">
         <v>0.1144677576102641</v>
       </c>
     </row>

</xml_diff>